<commit_message>
Removed stupid things from the diagram.
PACMAN-6
</commit_message>
<xml_diff>
--- a/Documents/GameEngineArchitecture.xlsx
+++ b/Documents/GameEngineArchitecture.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="19095" windowHeight="12270"/>
@@ -2620,53 +2620,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="sv-SE" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="93" name="Rounded Rectangle 92"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4026658" y="3429000"/>
-            <a:ext cx="1154942" cy="366346"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent5">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent5"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="sv-SE" sz="1100">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Heads-Up Display (HUD)</a:t>
-            </a:r>
+            <a:endParaRPr lang="sv-SE" sz="1100" i="1"/>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2721,7 +2675,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5550658" y="3429000"/>
+            <a:off x="4402555" y="3429000"/>
             <a:ext cx="850142" cy="366346"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
@@ -2780,7 +2734,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="6705600" y="3429000"/>
+            <a:off x="6233602" y="3429000"/>
             <a:ext cx="1219200" cy="366346"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
@@ -4087,14 +4041,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>265340</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>585108</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -4103,10 +4057,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="918483" y="2653393"/>
-          <a:ext cx="2932339" cy="952500"/>
-          <a:chOff x="16459200" y="3429000"/>
-          <a:chExt cx="2714625" cy="952500"/>
+          <a:off x="918483" y="2830286"/>
+          <a:ext cx="2932339" cy="816428"/>
+          <a:chOff x="16459200" y="3565072"/>
+          <a:chExt cx="2714625" cy="816428"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -4116,8 +4070,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="16459200" y="3429000"/>
-            <a:ext cx="2714625" cy="952500"/>
+            <a:off x="16459200" y="3565072"/>
+            <a:ext cx="2714625" cy="816428"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -4165,7 +4119,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="16828098" y="3810000"/>
+            <a:off x="16828098" y="3850821"/>
             <a:ext cx="850302" cy="366346"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
@@ -4211,7 +4165,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="18047298" y="3810000"/>
+            <a:off x="18085088" y="3864428"/>
             <a:ext cx="850302" cy="366346"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
@@ -4269,13 +4223,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>122465</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>149678</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>319767</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -4286,10 +4240,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3918857" y="2095500"/>
-          <a:ext cx="2932339" cy="1524000"/>
-          <a:chOff x="4252232" y="2095500"/>
-          <a:chExt cx="2932339" cy="1524000"/>
+          <a:off x="4041322" y="2816678"/>
+          <a:ext cx="3714750" cy="802822"/>
+          <a:chOff x="4252233" y="2816678"/>
+          <a:chExt cx="3714750" cy="802822"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -4299,10 +4253,10 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="4252232" y="2095500"/>
-            <a:ext cx="2932339" cy="1524000"/>
-            <a:chOff x="16459200" y="3429000"/>
-            <a:chExt cx="2714625" cy="1524000"/>
+            <a:off x="4252233" y="2816678"/>
+            <a:ext cx="3714750" cy="802822"/>
+            <a:chOff x="16459200" y="4150178"/>
+            <a:chExt cx="3438945" cy="802822"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -4312,8 +4266,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="16459200" y="3429000"/>
-              <a:ext cx="2714625" cy="1524000"/>
+              <a:off x="16459200" y="4150178"/>
+              <a:ext cx="3438945" cy="802822"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4361,7 +4315,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="16755227" y="3810000"/>
+              <a:off x="18858902" y="4449535"/>
               <a:ext cx="850302" cy="366346"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
@@ -4407,7 +4361,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17964526" y="3810000"/>
+              <a:off x="17800767" y="4449535"/>
               <a:ext cx="850302" cy="366346"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
@@ -4454,7 +4408,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4572000" y="3062654"/>
+            <a:off x="4572000" y="3117082"/>
             <a:ext cx="918497" cy="366346"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
@@ -4490,49 +4444,6 @@
               </a:rPr>
               <a:t>States</a:t>
             </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="139" name="Rounded Rectangle 138"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5878286" y="3062654"/>
-            <a:ext cx="918497" cy="366346"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent5">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent5"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="sv-SE" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -4691,16 +4602,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95252</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>319767</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571503</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>13607</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -4709,10 +4620,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7184571" y="2095500"/>
-          <a:ext cx="2932339" cy="1524000"/>
-          <a:chOff x="4252232" y="2095500"/>
-          <a:chExt cx="2932339" cy="1524000"/>
+          <a:off x="7932966" y="2803071"/>
+          <a:ext cx="4395108" cy="830036"/>
+          <a:chOff x="4252234" y="2789464"/>
+          <a:chExt cx="2932339" cy="830036"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -4722,10 +4633,10 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="4252232" y="2095500"/>
-            <a:ext cx="2932339" cy="1524000"/>
-            <a:chOff x="16459200" y="3429000"/>
-            <a:chExt cx="2714625" cy="1524000"/>
+            <a:off x="4252234" y="2789464"/>
+            <a:ext cx="2932339" cy="830036"/>
+            <a:chOff x="16459202" y="4122964"/>
+            <a:chExt cx="2714625" cy="830036"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -4735,8 +4646,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="16459200" y="3429000"/>
-              <a:ext cx="2714625" cy="1524000"/>
+              <a:off x="16459202" y="4122964"/>
+              <a:ext cx="2714625" cy="830036"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4784,8 +4695,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="16755227" y="3810000"/>
-              <a:ext cx="850302" cy="366346"/>
+              <a:off x="16570330" y="4449535"/>
+              <a:ext cx="662076" cy="366346"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
               <a:avLst/>
@@ -4843,8 +4754,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17964526" y="3810000"/>
-              <a:ext cx="850302" cy="366346"/>
+              <a:off x="18317511" y="4435928"/>
+              <a:ext cx="713438" cy="366346"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
               <a:avLst/>
@@ -4885,13 +4796,13 @@
       </xdr:grpSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="147" name="Rounded Rectangle 146"/>
+          <xdr:cNvPr id="148" name="Rounded Rectangle 147"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4572000" y="3062654"/>
-            <a:ext cx="918497" cy="366346"/>
+            <a:off x="5297265" y="3117082"/>
+            <a:ext cx="725264" cy="366346"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
             <a:avLst/>
@@ -4918,49 +4829,6 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="sv-SE" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="148" name="Rounded Rectangle 147"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5878286" y="3062654"/>
-            <a:ext cx="918497" cy="366346"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent5">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent5"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
             <a:r>
               <a:rPr lang="sv-SE" sz="1100">
                 <a:solidFill>
@@ -4977,16 +4845,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>14654</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>164332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>265355</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>455854</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>149678</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4995,7 +4863,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11103429" y="1729154"/>
+          <a:off x="5415643" y="2069332"/>
           <a:ext cx="918497" cy="366346"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -5038,16 +4906,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>14654</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>299357</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>164332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>265355</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>564711</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>149678</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5056,7 +4924,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11103429" y="2300654"/>
+          <a:off x="4218214" y="2069332"/>
           <a:ext cx="918497" cy="366346"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -5388,7 +5256,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V47" sqref="V47"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15"/>

</xml_diff>